<commit_message>
remove more obsolete code, add include folder for client
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2801BB81-6A9B-414C-8E32-2CE9F1AB2B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF196373-03A4-4A3C-873E-5859B9177412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>z_waves_port working (THEY COME FROM THE SEA/!?!?!?!?!) - z_tdm_spire finished</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Properly split out client.h, server.h</t>
   </si>
 </sst>
 </file>
@@ -447,31 +459,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2139B6D-D7BF-4635-BEFA-D5AA4E9A3D04}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="98.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,178 +496,85 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Increased console line length from 38 to 128 characters (this will be a CVar in the future)
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DC1B2E-C2BA-46F7-8E6B-71C3A7B87974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7723A846-FA8F-4212-8FB9-56EDC5E27D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="1935" windowWidth="12765" windowHeight="12120" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Allow people to see what team a player is</t>
+  </si>
+  <si>
+    <t>Make Master servers work</t>
+  </si>
+  <si>
+    <t>Feature, Netservuces</t>
+  </si>
+  <si>
+    <t>cl_console_line_length</t>
   </si>
 </sst>
 </file>
@@ -486,7 +495,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -570,24 +579,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -595,42 +604,54 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
increment version to 0.0.11
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7723A846-FA8F-4212-8FB9-56EDC5E27D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF788B3-2FBC-49D9-B240-D0171828EA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>cl_console_line_length</t>
+  </si>
+  <si>
+    <t>Fix game connecting to server during intro</t>
+  </si>
+  <si>
+    <t>Fix relatve velocity being added multiple times</t>
+  </si>
+  <si>
+    <t>func_train in subway fucked up</t>
+  </si>
+  <si>
+    <t>Fucked up chair collision</t>
+  </si>
+  <si>
+    <t>Zombification: you can get stuck</t>
+  </si>
+  <si>
+    <t>Green pipe, add poster there</t>
+  </si>
+  <si>
+    <t>Game does not clear entities on 2nd entry into a map</t>
   </si>
 </sst>
 </file>
@@ -492,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2139B6D-D7BF-4635-BEFA-D5AA4E9A3D04}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -547,64 +568,64 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -613,15 +634,15 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -629,7 +650,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -638,29 +659,83 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
limit relative velocity for non-rockets and non-tangfuslicators
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF788B3-2FBC-49D9-B240-D0171828EA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D51E90E-76BF-4134-BFA7-19F42FC23C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Make Master servers work</t>
   </si>
   <si>
-    <t>Feature, Netservuces</t>
-  </si>
-  <si>
     <t>cl_console_line_length</t>
   </si>
   <si>
@@ -145,6 +142,18 @@
   </si>
   <si>
     <t>Game does not clear entities on 2nd entry into a map</t>
+  </si>
+  <si>
+    <t>De-jankify tangfuslicator jump</t>
+  </si>
+  <si>
+    <t>Feature, Bugfix</t>
+  </si>
+  <si>
+    <t>Alt+tab crash in dedicated fullscreen</t>
+  </si>
+  <si>
+    <t>Incorrect update channel description (Release) being pulled on Debug</t>
   </si>
 </sst>
 </file>
@@ -513,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2139B6D-D7BF-4635-BEFA-D5AA4E9A3D04}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -568,7 +577,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
@@ -576,7 +585,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
@@ -584,7 +593,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -592,7 +601,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -600,7 +609,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -608,7 +617,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -617,7 +626,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -625,32 +634,32 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -659,25 +668,25 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -685,24 +694,24 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -710,7 +719,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
@@ -718,22 +727,46 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
split out gamemode specific code
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CFC3F5-5985-44BA-B31C-17DD320A00E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3408BD53-2072-4AAA-8523-0D47F10A2D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Fix relative velocity being added multiple times</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -185,12 +188,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -205,12 +214,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +538,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,6 +603,9 @@
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -641,6 +654,9 @@
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D12" s="3"/>
     </row>

</xml_diff>

<commit_message>
begin working on new master server protocol
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3408BD53-2072-4AAA-8523-0D47F10A2D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A43012D-5C2C-4226-AF6C-22D2F466D386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
+    <workbookView xWindow="4710" yWindow="2805" windowWidth="12975" windowHeight="12120" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Fix: Warehouse ramps too steep</t>
   </si>
   <si>
-    <t>Fix " velocity increasing but not speed" (prediction miss bug when hitting wall at specific angle sometimes)</t>
-  </si>
-  <si>
     <t>Complete Release Generation Tool</t>
   </si>
   <si>
@@ -120,46 +117,49 @@
     <t>cl_console_line_length</t>
   </si>
   <si>
-    <t>Fix game connecting to server during intro</t>
-  </si>
-  <si>
-    <t>func_train in subway fucked up</t>
-  </si>
-  <si>
-    <t>Fucked up chair collision</t>
-  </si>
-  <si>
-    <t>Zombification: you can get stuck</t>
-  </si>
-  <si>
-    <t>Green pipe, add poster there</t>
-  </si>
-  <si>
-    <t>Game does not clear entities on 2nd entry into a map</t>
-  </si>
-  <si>
     <t>De-jankify tangfuslicator jump</t>
   </si>
   <si>
     <t>Feature, Bugfix</t>
   </si>
   <si>
-    <t>Alt+tab crash in dedicated fullscreen</t>
-  </si>
-  <si>
-    <t>Incorrect update channel description (Release) being pulled on Debug</t>
-  </si>
-  <si>
     <t>Zombono v0.0.11 (could also be 0.1.0 if we finish anything)</t>
   </si>
   <si>
     <t>Gamemodes per-file</t>
   </si>
   <si>
-    <t>Fix relative velocity being added multiple times</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Fix: func_train in subway fucked up</t>
+  </si>
+  <si>
+    <t>Fix: Fucked up chair collision</t>
+  </si>
+  <si>
+    <t>Fix: relative velocity being added multiple times</t>
+  </si>
+  <si>
+    <t>Fix: game connecting to server during intro</t>
+  </si>
+  <si>
+    <t>Fix: "velocity increasing but not speed" (prediction miss bug when hitting wall at specific angle sometimes)</t>
+  </si>
+  <si>
+    <t>Fix: Zombification: you can get stuck</t>
+  </si>
+  <si>
+    <t>Fix: Incorrect update channel description (Release) being pulled on Debug</t>
+  </si>
+  <si>
+    <t>Fix: Alt+tab crash in dedicated fullscreen</t>
+  </si>
+  <si>
+    <t>Fix: Game does not clear entities on 2nd entry into a map</t>
+  </si>
+  <si>
+    <t>Fix:  Green pipe, add poster there</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -552,7 +552,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -577,103 +577,103 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
@@ -705,15 +705,15 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
move anorms.h to include
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13031377-CA5A-411C-AC71-136FCDAAE082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E505F9B-F97B-4FE2-B660-E5327A2A9D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A41" sqref="A40:A41"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -629,6 +629,9 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fully reorganise client code
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12924662-44A6-44F1-8179-73E00837B6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4DE4DC-41E5-4B59-AEFE-F955BE9C06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2139B6D-D7BF-4635-BEFA-D5AA4E9A3D04}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -600,6 +600,9 @@
       <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="D6" s="3">
+        <v>45454</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -635,7 +638,9 @@
       <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>45456</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -655,7 +660,9 @@
       <c r="C12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3">
+        <v>45454</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">

</xml_diff>

<commit_message>
s_volume -> s_volume_sfx, automatic rescaling, ui stack
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.11.xlsx
+++ b/docs/version_scheduling/0.0.11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4DE4DC-41E5-4B59-AEFE-F955BE9C06D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942A34BD-0148-41E5-A33D-7219B74E0DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -531,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2139B6D-D7BF-4635-BEFA-D5AA4E9A3D04}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>